<commit_message>
dev-61 - fixed upload tt for many employees
</commit_message>
<xml_diff>
--- a/etc/scripts/timetable.xlsx
+++ b/etc/scripts/timetable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="30">
   <si>
     <t>Номер</t>
   </si>
@@ -112,10 +112,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -153,6 +153,126 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -161,74 +281,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -237,51 +289,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,13 +296,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -318,187 +318,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,11 +542,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,21 +629,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -630,130 +639,121 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -762,28 +762,28 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1155,7 +1155,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="15.75"/>
@@ -1809,7 +1809,107 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="35" customHeight="true"/>
+    <row r="7" ht="35" customHeight="true" spans="1:33">
+      <c r="A7" s="3">
+        <v>26856</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="8" ht="20" customHeight="true"/>
     <row r="9" ht="20" customHeight="true"/>
     <row r="10" ht="20" customHeight="true" spans="2:2">

</xml_diff>

<commit_message>
rnd-176 - added test for upload
</commit_message>
<xml_diff>
--- a/etc/scripts/timetable.xlsx
+++ b/etc/scripts/timetable.xlsx
@@ -1,17 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anton/QoS_backend/etc/scripts/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581A4CF0-10DA-FB4A-B083-97A24791CFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-9680" yWindow="-21080" windowWidth="48640" windowHeight="21080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Расписание на подпись" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Расписание на подпись" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -20,178 +35,190 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="35">
-  <si>
-    <t xml:space="preserve">Номер</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ФИО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ДОЛЖНОСТЬ</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="42">
+  <si>
+    <t>Номер</t>
+  </si>
+  <si>
+    <t>ФИО</t>
+  </si>
+  <si>
+    <t>ДОЛЖНОСТЬ</t>
   </si>
   <si>
     <t xml:space="preserve"> A23739 </t>
   </si>
   <si>
-    <t xml:space="preserve">Иванов Иван Иванович</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Директор магазина</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:0-20:0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">В</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00.20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28479</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Петров Петр Петрович</t>
-  </si>
-  <si>
-    <t xml:space="preserve">продавец</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00, 20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00 20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27665</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сидоров Сергей Сергеевич</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Продавец-кассир</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-14:00/18:00-20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">К10:00-21:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27511</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Аленова Алена Аленовна</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Продавец</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-20:0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00
+    <t>Иванов Иван Иванович</t>
+  </si>
+  <si>
+    <t>Директор магазина</t>
+  </si>
+  <si>
+    <t>10:0-20:0</t>
+  </si>
+  <si>
+    <t>10:00-20:00</t>
+  </si>
+  <si>
+    <t>В</t>
+  </si>
+  <si>
+    <t>10:00.20:00</t>
+  </si>
+  <si>
+    <t>28479</t>
+  </si>
+  <si>
+    <t>Петров Петр Петрович</t>
+  </si>
+  <si>
+    <t>продавец</t>
+  </si>
+  <si>
+    <t>10:00, 20:00</t>
+  </si>
+  <si>
+    <t>10:00 20:00</t>
+  </si>
+  <si>
+    <t>27665</t>
+  </si>
+  <si>
+    <t>Сидоров Сергей Сергеевич</t>
+  </si>
+  <si>
+    <t>Продавец-кассир</t>
+  </si>
+  <si>
+    <t>10:00-14:00/18:00-20:00</t>
+  </si>
+  <si>
+    <t>К10:00-21:00</t>
+  </si>
+  <si>
+    <t>27511</t>
+  </si>
+  <si>
+    <t>Аленова Алена Аленовна</t>
+  </si>
+  <si>
+    <t>Продавец</t>
+  </si>
+  <si>
+    <t>10:00-20:0</t>
+  </si>
+  <si>
+    <t>10:00
 20:00</t>
   </si>
   <si>
-    <t xml:space="preserve">26855</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Смешнов Александр Николаевич</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ЗДМ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00,20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* первая строка содержит название столбцов: номер сотрудника, ФИО, его должность, далее даты, для которых указывается плановый график сотрудника</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* при загрузки списка сотрудников достаточно заполнить первые 3 столбца (даты нет необходимости указывать</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Для указания работы сотрудника в определнный день указывается время начало смены, дефис, время окончания работы (например, 10:00 - 19:30)</t>
+    <t>26855</t>
+  </si>
+  <si>
+    <t>Смешнов Александр Николаевич</t>
+  </si>
+  <si>
+    <t>ЗДМ</t>
+  </si>
+  <si>
+    <t>10:00,20:00</t>
+  </si>
+  <si>
+    <t>* первая строка содержит название столбцов: номер сотрудника, ФИО, его должность, далее даты, для которых указывается плановый график сотрудника</t>
+  </si>
+  <si>
+    <t>* при загрузки списка сотрудников достаточно заполнить первые 3 столбца (даты нет необходимости указывать</t>
+  </si>
+  <si>
+    <t>* Для указания работы сотрудника в определнный день указывается время начало смены, дефис, время окончания работы (например, 10:00 - 19:30)</t>
   </si>
   <si>
     <t xml:space="preserve">* для указания выходного, отпуска или другого статуса рабочего используется русская буква В </t>
   </si>
   <si>
-    <t xml:space="preserve">* форматирование (цвет ячейки, жирность текста, шрифт и тд) не играет роли при загрузке данных</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* даты должны идти подряд (без пропусков)</t>
+    <t>* форматирование (цвет ячейки, жирность текста, шрифт и тд) не играет роли при загрузке данных</t>
+  </si>
+  <si>
+    <t>* даты должны идти подряд (без пропусков)</t>
+  </si>
+  <si>
+    <t>~10:00-20:00</t>
+  </si>
+  <si>
+    <t>~10:00-20:00 (ДМ)</t>
+  </si>
+  <si>
+    <t>10:00-20:00 (Non existent)</t>
+  </si>
+  <si>
+    <t>10:00-20:00 (ДМ)</t>
+  </si>
+  <si>
+    <t>10:00-20:00(Кассы)</t>
+  </si>
+  <si>
+    <t>Б10.0</t>
+  </si>
+  <si>
+    <t>Б  10,0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="h:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="h:mm:ss"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,124 +237,421 @@
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+  <a:themeElements>
+    <a:clrScheme name="Стандартная">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Стандартная">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Стандартная">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AG15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BO15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="12" style="0" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="67" min="58" style="0" width="3.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="68" style="0" width="15.17"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
+    <col min="8" max="10" width="10.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="12" max="15" width="10.1640625" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="18" max="33" width="10.1640625" customWidth="1"/>
+    <col min="58" max="67" width="3.83203125" hidden="1" customWidth="1"/>
+    <col min="68" max="71" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -337,127 +661,127 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="n">
+      <c r="D1" s="2">
         <v>43922</v>
       </c>
-      <c r="E1" s="2" t="n">
-        <f aca="false">D1+1</f>
+      <c r="E1" s="2">
+        <f t="shared" ref="E1:AG1" si="0">D1+1</f>
         <v>43923</v>
       </c>
-      <c r="F1" s="2" t="n">
-        <f aca="false">E1+1</f>
+      <c r="F1" s="2">
+        <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="G1" s="2" t="n">
-        <f aca="false">F1+1</f>
+      <c r="G1" s="2">
+        <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="H1" s="2" t="n">
-        <f aca="false">G1+1</f>
+      <c r="H1" s="2">
+        <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="I1" s="2" t="n">
-        <f aca="false">H1+1</f>
+      <c r="I1" s="2">
+        <f t="shared" si="0"/>
         <v>43927</v>
       </c>
-      <c r="J1" s="2" t="n">
-        <f aca="false">I1+1</f>
+      <c r="J1" s="2">
+        <f t="shared" si="0"/>
         <v>43928</v>
       </c>
-      <c r="K1" s="2" t="n">
-        <f aca="false">J1+1</f>
+      <c r="K1" s="2">
+        <f t="shared" si="0"/>
         <v>43929</v>
       </c>
-      <c r="L1" s="2" t="n">
-        <f aca="false">K1+1</f>
+      <c r="L1" s="2">
+        <f t="shared" si="0"/>
         <v>43930</v>
       </c>
-      <c r="M1" s="2" t="n">
-        <f aca="false">L1+1</f>
+      <c r="M1" s="2">
+        <f t="shared" si="0"/>
         <v>43931</v>
       </c>
-      <c r="N1" s="2" t="n">
-        <f aca="false">M1+1</f>
+      <c r="N1" s="2">
+        <f t="shared" si="0"/>
         <v>43932</v>
       </c>
-      <c r="O1" s="2" t="n">
-        <f aca="false">N1+1</f>
+      <c r="O1" s="2">
+        <f t="shared" si="0"/>
         <v>43933</v>
       </c>
-      <c r="P1" s="2" t="n">
-        <f aca="false">O1+1</f>
+      <c r="P1" s="2">
+        <f t="shared" si="0"/>
         <v>43934</v>
       </c>
-      <c r="Q1" s="2" t="n">
-        <f aca="false">P1+1</f>
+      <c r="Q1" s="2">
+        <f t="shared" si="0"/>
         <v>43935</v>
       </c>
-      <c r="R1" s="2" t="n">
-        <f aca="false">Q1+1</f>
+      <c r="R1" s="2">
+        <f t="shared" si="0"/>
         <v>43936</v>
       </c>
-      <c r="S1" s="2" t="n">
-        <f aca="false">R1+1</f>
+      <c r="S1" s="2">
+        <f t="shared" si="0"/>
         <v>43937</v>
       </c>
-      <c r="T1" s="2" t="n">
-        <f aca="false">S1+1</f>
+      <c r="T1" s="2">
+        <f t="shared" si="0"/>
         <v>43938</v>
       </c>
-      <c r="U1" s="2" t="n">
-        <f aca="false">T1+1</f>
+      <c r="U1" s="2">
+        <f t="shared" si="0"/>
         <v>43939</v>
       </c>
-      <c r="V1" s="2" t="n">
-        <f aca="false">U1+1</f>
+      <c r="V1" s="2">
+        <f t="shared" si="0"/>
         <v>43940</v>
       </c>
-      <c r="W1" s="2" t="n">
-        <f aca="false">V1+1</f>
+      <c r="W1" s="2">
+        <f t="shared" si="0"/>
         <v>43941</v>
       </c>
-      <c r="X1" s="2" t="n">
-        <f aca="false">W1+1</f>
+      <c r="X1" s="2">
+        <f t="shared" si="0"/>
         <v>43942</v>
       </c>
-      <c r="Y1" s="2" t="n">
-        <f aca="false">X1+1</f>
+      <c r="Y1" s="2">
+        <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="Z1" s="2" t="n">
-        <f aca="false">Y1+1</f>
+      <c r="Z1" s="2">
+        <f t="shared" si="0"/>
         <v>43944</v>
       </c>
-      <c r="AA1" s="2" t="n">
-        <f aca="false">Z1+1</f>
+      <c r="AA1" s="2">
+        <f t="shared" si="0"/>
         <v>43945</v>
       </c>
-      <c r="AB1" s="2" t="n">
-        <f aca="false">AA1+1</f>
+      <c r="AB1" s="2">
+        <f t="shared" si="0"/>
         <v>43946</v>
       </c>
-      <c r="AC1" s="2" t="n">
-        <f aca="false">AB1+1</f>
+      <c r="AC1" s="2">
+        <f t="shared" si="0"/>
         <v>43947</v>
       </c>
-      <c r="AD1" s="2" t="n">
-        <f aca="false">AC1+1</f>
+      <c r="AD1" s="2">
+        <f t="shared" si="0"/>
         <v>43948</v>
       </c>
-      <c r="AE1" s="2" t="n">
-        <f aca="false">AD1+1</f>
+      <c r="AE1" s="2">
+        <f t="shared" si="0"/>
         <v>43949</v>
       </c>
-      <c r="AF1" s="2" t="n">
-        <f aca="false">AE1+1</f>
+      <c r="AF1" s="2">
+        <f t="shared" si="0"/>
         <v>43950</v>
       </c>
-      <c r="AG1" s="2" t="n">
-        <f aca="false">AF1+1</f>
+      <c r="AG1" s="2">
+        <f t="shared" si="0"/>
         <v>43951</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:33" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -504,10 +828,10 @@
         <v>8</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>7</v>
+        <v>36</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>7</v>
@@ -558,7 +882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:33" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -608,7 +932,7 @@
         <v>8</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>7</v>
@@ -659,7 +983,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:33" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -708,11 +1032,11 @@
       <c r="P4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>8</v>
+      <c r="Q4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>8</v>
@@ -760,7 +1084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:33" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -807,7 +1131,7 @@
         <v>8</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>7</v>
@@ -861,7 +1185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:33" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -962,8 +1286,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+    <row r="7" spans="1:33" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>26856</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1012,7 +1336,7 @@
         <v>7</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>7</v>
@@ -1063,45 +1387,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+    <row r="8" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+    <row r="11" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+    <row r="12" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>